<commit_message>
Estimate time for task + submit effort log week 16
</commit_message>
<xml_diff>
--- a/DELIVERABLE/EFFORT_LOG/Week16/BSS_EffortLog_MinhDoan_Week16.xlsx
+++ b/DELIVERABLE/EFFORT_LOG/Week16/BSS_EffortLog_MinhDoan_Week16.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CapstonProject\CapstonProject\TEMPLATE\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,12 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">EFFORT LOG </t>
-  </si>
-  <si>
-    <t>WEEK:</t>
   </si>
   <si>
     <t>No.</t>
@@ -49,11 +41,23 @@
   <si>
     <t>Actual Time</t>
   </si>
+  <si>
+    <t>Demo Function "Create Draft" using Angular2 , Mongodb</t>
+  </si>
+  <si>
+    <t>WEEK:16</t>
+  </si>
+  <si>
+    <t>19/1/2017</t>
+  </si>
+  <si>
+    <t>20/1/2017</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -136,13 +140,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -150,6 +148,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -210,7 +214,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -262,7 +266,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -456,7 +460,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -467,32 +471,33 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8" style="4" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" style="4" customWidth="1"/>
-    <col min="4" max="5" width="8.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="9" style="4" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" style="4" customWidth="1"/>
-    <col min="9" max="27" width="7.5703125" style="4" customWidth="1"/>
-    <col min="28" max="16384" width="15.140625" style="4"/>
+    <col min="1" max="2" width="8" style="3" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="50.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="3" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="3" customWidth="1"/>
+    <col min="9" max="27" width="7.5703125" style="3" customWidth="1"/>
+    <col min="28" max="16384" width="15.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -516,14 +521,14 @@
     <row r="2" spans="1:27" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="5" t="s">
-        <v>1</v>
+      <c r="C2" s="10" t="s">
+        <v>8</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -574,55 +579,67 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="6"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="6">
+        <v>6</v>
+      </c>
+      <c r="H5" s="6">
+        <v>5</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -646,12 +663,12 @@
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -675,12 +692,12 @@
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -704,12 +721,12 @@
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -733,12 +750,12 @@
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -762,12 +779,12 @@
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -791,12 +808,12 @@
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -820,12 +837,12 @@
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -849,12 +866,12 @@
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -878,12 +895,12 @@
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>

</xml_diff>